<commit_message>
Update Run as FireFox
</commit_message>
<xml_diff>
--- a/src/test/resources/Boo.xlsx
+++ b/src/test/resources/Boo.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="85">
   <si>
     <t/>
   </si>
@@ -275,6 +275,42 @@
   </si>
   <si>
     <t>b) 1, 4, 5, 6</t>
+  </si>
+  <si>
+    <t>Question 8:</t>
+  </si>
+  <si>
+    <t>Question #8
+Match the following test work products (1-4) with the right description (A-D).
+1. Test suite.
+2. Test case.
+3. Test script.
+4. Test charter.
+A. A set of test scripts to be executed in a specific test run.
+B. A set of instructions for the execution of a test.
+C. Contains expected results.
+D. Documentation of test activities in session-based exploratory testing.</t>
+  </si>
+  <si>
+    <t>Match the following test work products (1-4) with the right description (A-D).</t>
+  </si>
+  <si>
+    <t>a) 1A, 2C, 3B, 4D.</t>
+  </si>
+  <si>
+    <t>b) 1D, 2B, 3A, 4C.</t>
+  </si>
+  <si>
+    <t>c) 1A, 2C, 3D, 4B.</t>
+  </si>
+  <si>
+    <t>d) 1D, 2C, 3B, 4A.</t>
+  </si>
+  <si>
+    <t>c) 2, 3, 4, 5</t>
+  </si>
+  <si>
+    <t>d) 3, 5, 6</t>
   </si>
 </sst>
 </file>
@@ -605,7 +641,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1181,6 +1217,81 @@
         <v>70</v>
       </c>
     </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54"/>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" t="s">
+        <v>77</v>
+      </c>
+      <c r="C55" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>76</v>
+      </c>
+      <c r="B59" t="s">
+        <v>77</v>
+      </c>
+      <c r="C59" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1188,7 +1299,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1353,6 +1464,81 @@
       </c>
       <c r="C15" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17"/>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>